<commit_message>
Player status at the end of the 7-13 March week
</commit_message>
<xml_diff>
--- a/player-status.xlsx
+++ b/player-status.xlsx
@@ -44,14 +44,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,12 +113,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,7 +143,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -145,11 +151,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -171,13 +178,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>700</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <f aca="false">C2/D2</f>
+        <v>0.928571428571429</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,22 +196,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>295</v>
+        <v>375</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>500</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <f aca="false">C3/D3</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <f aca="false">B3/B2</f>
+        <v>0.744047619047619</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">C3/C2</f>
+        <v>0.692307692307692</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">D3/D2</f>
+        <v>0.714285714285714</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Pàgina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pàgina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Save into DB missing players
</commit_message>
<xml_diff>
--- a/player-status.xlsx
+++ b/player-status.xlsx
@@ -190,7 +190,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>650</v>
+        <v>676</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>700</v>
@@ -200,7 +200,7 @@
       </c>
       <c r="E2" s="2" t="n">
         <f aca="false">B2/C2</f>
-        <v>0.928571428571429</v>
+        <v>0.965714285714286</v>
       </c>
       <c r="F2" s="2" t="n">
         <f aca="false">C2/D2</f>
@@ -232,7 +232,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <f aca="false">(B3/B2)/0.75</f>
-        <v>0.925128205128205</v>
+        <v>0.889546351084813</v>
       </c>
       <c r="C4" s="2" t="n">
         <f aca="false">(C3/C2)/0.75</f>
@@ -246,10 +246,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Pàgina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pàgina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>